<commit_message>
updated file extensions and forecasting
</commit_message>
<xml_diff>
--- a/food_security_forecasting/data/Nutritional_Programming_West.xlsx
+++ b/food_security_forecasting/data/Nutritional_Programming_West.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/goldencami/Desktop/GitHub/ConcordIA/food_security_forecasting/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DF4D686-707D-0345-A25D-DABBDB83A83B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9CD226-E6E2-2748-A3FF-FB1F0C54D46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3660" yWindow="2660" windowWidth="27640" windowHeight="16940" xr2:uid="{4E9F38FD-C26A-5E46-8B87-780FEEFAD7D6}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{4E9F38FD-C26A-5E46-8B87-780FEEFAD7D6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1979,9 +1979,6 @@
     <t>Property Notes_YD</t>
   </si>
   <si>
-    <t>MemberFN_YD</t>
-  </si>
-  <si>
     <t>MemberLN_YD</t>
   </si>
   <si>
@@ -2217,6 +2214,9 @@
   </si>
   <si>
     <t>Encounter Status_TR</t>
+  </si>
+  <si>
+    <t>MemberFN_YD+DH1</t>
   </si>
 </sst>
 </file>
@@ -2672,8 +2672,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82747B68-FE52-C548-B72B-EF34C2C8F4AC}">
   <dimension ref="A1:GF91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="FU61" workbookViewId="0">
-      <selection activeCell="FY66" sqref="FY66"/>
+    <sheetView tabSelected="1" topLeftCell="FT1" workbookViewId="0">
+      <selection activeCell="FV1" sqref="FV1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3074,244 +3074,244 @@
         <v>646</v>
       </c>
       <c r="DE1" s="5" t="s">
+        <v>726</v>
+      </c>
+      <c r="DF1" s="5" t="s">
         <v>647</v>
       </c>
-      <c r="DF1" s="5" t="s">
+      <c r="DG1" s="5" t="s">
         <v>648</v>
       </c>
-      <c r="DG1" s="5" t="s">
+      <c r="DH1" s="5" t="s">
         <v>649</v>
       </c>
-      <c r="DH1" s="5" t="s">
+      <c r="DI1" s="5" t="s">
         <v>650</v>
       </c>
-      <c r="DI1" s="5" t="s">
+      <c r="DJ1" s="5" t="s">
         <v>651</v>
       </c>
-      <c r="DJ1" s="5" t="s">
+      <c r="DK1" s="5" t="s">
         <v>652</v>
       </c>
-      <c r="DK1" s="5" t="s">
+      <c r="DL1" s="5" t="s">
         <v>653</v>
       </c>
-      <c r="DL1" s="5" t="s">
+      <c r="DM1" s="5" t="s">
         <v>654</v>
       </c>
-      <c r="DM1" s="5" t="s">
+      <c r="DN1" s="5" t="s">
         <v>655</v>
       </c>
-      <c r="DN1" s="5" t="s">
+      <c r="DO1" s="5" t="s">
         <v>656</v>
       </c>
-      <c r="DO1" s="5" t="s">
+      <c r="DP1" s="5" t="s">
         <v>657</v>
       </c>
-      <c r="DP1" s="5" t="s">
+      <c r="DQ1" s="5" t="s">
         <v>658</v>
       </c>
-      <c r="DQ1" s="5" t="s">
+      <c r="DR1" s="5" t="s">
         <v>659</v>
       </c>
-      <c r="DR1" s="5" t="s">
+      <c r="DS1" s="5" t="s">
         <v>660</v>
       </c>
-      <c r="DS1" s="5" t="s">
+      <c r="DT1" s="5" t="s">
         <v>661</v>
       </c>
-      <c r="DT1" s="5" t="s">
+      <c r="DU1" s="5" t="s">
         <v>662</v>
       </c>
-      <c r="DU1" s="5" t="s">
+      <c r="DV1" s="5" t="s">
         <v>663</v>
       </c>
-      <c r="DV1" s="5" t="s">
+      <c r="DW1" s="5" t="s">
         <v>664</v>
       </c>
-      <c r="DW1" s="5" t="s">
+      <c r="DX1" s="5" t="s">
         <v>665</v>
       </c>
-      <c r="DX1" s="5" t="s">
+      <c r="DY1" s="5" t="s">
         <v>666</v>
       </c>
-      <c r="DY1" s="5" t="s">
+      <c r="DZ1" s="5" t="s">
         <v>667</v>
       </c>
-      <c r="DZ1" s="5" t="s">
+      <c r="EA1" s="5" t="s">
         <v>668</v>
       </c>
-      <c r="EA1" s="5" t="s">
+      <c r="EB1" s="8" t="s">
         <v>669</v>
       </c>
-      <c r="EB1" s="8" t="s">
+      <c r="EC1" s="5" t="s">
         <v>670</v>
       </c>
-      <c r="EC1" s="5" t="s">
+      <c r="ED1" s="5" t="s">
         <v>671</v>
       </c>
-      <c r="ED1" s="5" t="s">
+      <c r="EE1" s="5" t="s">
         <v>672</v>
       </c>
-      <c r="EE1" s="5" t="s">
+      <c r="EF1" s="5" t="s">
         <v>673</v>
       </c>
-      <c r="EF1" s="5" t="s">
+      <c r="EG1" s="5" t="s">
         <v>674</v>
       </c>
-      <c r="EG1" s="5" t="s">
+      <c r="EH1" s="6" t="s">
         <v>675</v>
       </c>
-      <c r="EH1" s="6" t="s">
+      <c r="EI1" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="EI1" s="5" t="s">
+      <c r="EJ1" s="5" t="s">
         <v>677</v>
       </c>
-      <c r="EJ1" s="5" t="s">
+      <c r="EK1" s="5" t="s">
         <v>678</v>
       </c>
-      <c r="EK1" s="5" t="s">
+      <c r="EL1" s="5" t="s">
         <v>679</v>
       </c>
-      <c r="EL1" s="5" t="s">
+      <c r="EM1" s="5" t="s">
         <v>680</v>
       </c>
-      <c r="EM1" s="5" t="s">
+      <c r="EN1" s="5" t="s">
         <v>681</v>
       </c>
-      <c r="EN1" s="5" t="s">
+      <c r="EO1" s="5" t="s">
         <v>682</v>
       </c>
-      <c r="EO1" s="5" t="s">
+      <c r="EP1" s="5" t="s">
         <v>683</v>
       </c>
-      <c r="EP1" s="5" t="s">
+      <c r="EQ1" s="6" t="s">
         <v>684</v>
       </c>
-      <c r="EQ1" s="6" t="s">
+      <c r="ER1" s="5" t="s">
         <v>685</v>
       </c>
-      <c r="ER1" s="5" t="s">
+      <c r="ES1" s="5" t="s">
         <v>686</v>
       </c>
-      <c r="ES1" s="5" t="s">
+      <c r="ET1" s="6" t="s">
         <v>687</v>
       </c>
-      <c r="ET1" s="6" t="s">
+      <c r="EU1" s="5" t="s">
         <v>688</v>
       </c>
-      <c r="EU1" s="5" t="s">
+      <c r="EV1" s="5" t="s">
         <v>689</v>
       </c>
-      <c r="EV1" s="5" t="s">
+      <c r="EW1" s="6" t="s">
         <v>690</v>
       </c>
-      <c r="EW1" s="6" t="s">
+      <c r="EX1" s="5" t="s">
         <v>691</v>
       </c>
-      <c r="EX1" s="5" t="s">
+      <c r="EY1" s="5" t="s">
         <v>692</v>
       </c>
-      <c r="EY1" s="5" t="s">
+      <c r="EZ1" s="5" t="s">
         <v>693</v>
       </c>
-      <c r="EZ1" s="5" t="s">
+      <c r="FA1" s="5" t="s">
         <v>694</v>
       </c>
-      <c r="FA1" s="5" t="s">
+      <c r="FB1" s="5" t="s">
         <v>695</v>
       </c>
-      <c r="FB1" s="5" t="s">
+      <c r="FC1" s="5" t="s">
         <v>696</v>
       </c>
-      <c r="FC1" s="5" t="s">
+      <c r="FD1" s="5" t="s">
         <v>697</v>
       </c>
-      <c r="FD1" s="5" t="s">
+      <c r="FE1" s="5" t="s">
         <v>698</v>
       </c>
-      <c r="FE1" s="5" t="s">
+      <c r="FF1" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="FF1" s="5" t="s">
+      <c r="FG1" s="5" t="s">
         <v>700</v>
       </c>
-      <c r="FG1" s="5" t="s">
+      <c r="FH1" s="5" t="s">
         <v>701</v>
       </c>
-      <c r="FH1" s="5" t="s">
+      <c r="FI1" s="5" t="s">
         <v>702</v>
       </c>
-      <c r="FI1" s="5" t="s">
+      <c r="FJ1" s="6" t="s">
         <v>703</v>
       </c>
-      <c r="FJ1" s="6" t="s">
+      <c r="FK1" s="6" t="s">
         <v>704</v>
       </c>
-      <c r="FK1" s="6" t="s">
+      <c r="FL1" s="6" t="s">
         <v>705</v>
       </c>
-      <c r="FL1" s="6" t="s">
+      <c r="FM1" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="FM1" s="5" t="s">
+      <c r="FN1" s="5" t="s">
         <v>707</v>
       </c>
-      <c r="FN1" s="5" t="s">
+      <c r="FO1" s="5" t="s">
         <v>708</v>
       </c>
-      <c r="FO1" s="5" t="s">
+      <c r="FP1" s="5" t="s">
         <v>709</v>
       </c>
-      <c r="FP1" s="5" t="s">
+      <c r="FQ1" s="5" t="s">
         <v>710</v>
       </c>
-      <c r="FQ1" s="5" t="s">
+      <c r="FR1" s="5" t="s">
         <v>711</v>
       </c>
-      <c r="FR1" s="5" t="s">
+      <c r="FS1" s="5" t="s">
         <v>712</v>
       </c>
-      <c r="FS1" s="5" t="s">
+      <c r="FT1" s="5" t="s">
         <v>713</v>
       </c>
-      <c r="FT1" s="5" t="s">
+      <c r="FU1" s="5" t="s">
         <v>714</v>
       </c>
-      <c r="FU1" s="5" t="s">
+      <c r="FV1" s="5" t="s">
         <v>715</v>
       </c>
-      <c r="FV1" s="5" t="s">
+      <c r="FW1" s="6" t="s">
         <v>716</v>
       </c>
-      <c r="FW1" s="6" t="s">
+      <c r="FX1" s="5" t="s">
         <v>717</v>
       </c>
-      <c r="FX1" s="5" t="s">
+      <c r="FY1" s="5" t="s">
         <v>718</v>
       </c>
-      <c r="FY1" s="5" t="s">
+      <c r="FZ1" s="5" t="s">
         <v>719</v>
       </c>
-      <c r="FZ1" s="5" t="s">
+      <c r="GA1" s="6" t="s">
         <v>720</v>
       </c>
-      <c r="GA1" s="6" t="s">
+      <c r="GB1" s="5" t="s">
         <v>721</v>
       </c>
-      <c r="GB1" s="5" t="s">
+      <c r="GC1" s="5" t="s">
         <v>722</v>
       </c>
-      <c r="GC1" s="5" t="s">
+      <c r="GD1" s="5" t="s">
         <v>723</v>
       </c>
-      <c r="GD1" s="5" t="s">
+      <c r="GE1" s="6" t="s">
         <v>724</v>
       </c>
-      <c r="GE1" s="6" t="s">
+      <c r="GF1" s="5" t="s">
         <v>725</v>
-      </c>
-      <c r="GF1" s="5" t="s">
-        <v>726</v>
       </c>
     </row>
     <row r="2" spans="1:188" x14ac:dyDescent="0.2">

</xml_diff>